<commit_message>
Added algebra and changed dfd in report
</commit_message>
<xml_diff>
--- a/Алгебра.xlsx
+++ b/Алгебра.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fakyring\Desktop\МИРЭА\Курс 2\Проектирование БД\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B129398B-7452-43FB-B0A1-97499E983D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF067EEA-5CEE-4316-8391-118929BCB8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
   <si>
     <t>ID Сотрудника</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I8" sqref="I8:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,16 +441,20 @@
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -508,25 +512,25 @@
         <v>1</v>
       </c>
       <c r="I2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="M2" s="2">
-        <v>37186</v>
+        <v>37328</v>
       </c>
       <c r="N2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -546,25 +550,25 @@
         <v>3</v>
       </c>
       <c r="I3" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="M3" s="2">
-        <v>37092</v>
+        <v>4859</v>
       </c>
       <c r="N3" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -583,26 +587,8 @@
       <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="I4" s="1">
-        <v>3</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="2">
-        <v>37328</v>
-      </c>
-      <c r="N4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -621,26 +607,8 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="I5" s="1">
-        <v>4</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="2">
-        <v>4859</v>
-      </c>
-      <c r="N5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -650,8 +618,32 @@
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -661,8 +653,32 @@
       <c r="C9" s="1">
         <v>130000</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="2">
+        <v>37186</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="1">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -672,8 +688,32 @@
       <c r="C10" s="1">
         <v>70000</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="2">
+        <v>37092</v>
+      </c>
+      <c r="N10" s="1">
+        <v>3</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P10" s="1">
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -682,6 +722,56 @@
       </c>
       <c r="C11" s="1">
         <v>65000</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="2">
+        <v>37328</v>
+      </c>
+      <c r="N11" s="1">
+        <v>2</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="1">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I12" s="1">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="2">
+        <v>4859</v>
+      </c>
+      <c r="N12" s="1">
+        <v>2</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="1">
+        <v>70000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>